<commit_message>
renamed:    despachar_pedidos/main.py -> despachar_pedidos/core.py new file:   despachar_pedidos/interface.py modified:   despachar_pedidos/pedidos_x_notas.xlsx new file:   despachar_pedidos/tratamento_planilha.py modified:   utils/utils.py
</commit_message>
<xml_diff>
--- a/despachar_pedidos/pedidos_x_notas.xlsx
+++ b/despachar_pedidos/pedidos_x_notas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joab.alves\Desktop\automacoes_atacadao\despachar_pedidos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D762844C-88A8-4384-B263-E45DA90BF2FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C3345C-F7BC-4024-AAE3-2F2B3ABB6765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EF684577-2197-44B2-B2A3-F948CF0CE012}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Pedido</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>16005</t>
+  </si>
+  <si>
+    <t>teste</t>
+  </si>
+  <si>
+    <t>notaaa</t>
   </si>
 </sst>
 </file>
@@ -434,7 +440,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED1C1F2-75DA-4B52-BF29-FEEDB6E4B737}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -458,12 +466,20 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+      <c r="A4" s="2">
+        <v>17188</v>
+      </c>
+      <c r="B4" s="2">
+        <v>6377</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>

</xml_diff>